<commit_message>
hardware clients et instance clients
</commit_message>
<xml_diff>
--- a/src/loadFiles/update company/CI virtual Z.xlsx
+++ b/src/loadFiles/update company/CI virtual Z.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jdb\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3222F1FB-5814-4CFE-8B86-472AAF6ABB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3222F1FB-5814-4CFE-8B86-472AAF6ABB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,6 +48,9 @@
     <t>COMPANY</t>
   </si>
   <si>
+    <t>COMPANY_BREAKDOWN</t>
+  </si>
+  <si>
     <t>NRB_MANAGED_BY</t>
   </si>
   <si>
@@ -171,6 +174,9 @@
     <t>Z_GIAL03</t>
   </si>
   <si>
+    <t>RESA,IPEX,NRB</t>
+  </si>
+  <si>
     <t>z/OS - Production Mutualisée Resa, IPEX, …</t>
   </si>
   <si>
@@ -183,6 +189,9 @@
     <t>Z_GICH03</t>
   </si>
   <si>
+    <t>ETHIAS,PROVINCE LIEGE,AME-LIFE,NRB</t>
+  </si>
+  <si>
     <t>z/OS - Production Mutualisée batch &amp; java</t>
   </si>
   <si>
@@ -210,6 +219,9 @@
     <t>Z_GIDE03</t>
   </si>
   <si>
+    <t>ETHIAS,RESA,SIBELGA,PROVINCE LIEGE,AME-LIFE,NRB</t>
+  </si>
+  <si>
     <t>1.Développement</t>
   </si>
   <si>
@@ -252,6 +264,9 @@
     <t>Z_GIMVS</t>
   </si>
   <si>
+    <t>ETHIAS,RESA,PROVINCE LIEGE,AME-LIFE,NRB</t>
+  </si>
+  <si>
     <t>z/OS - Production mutualisée</t>
   </si>
   <si>
@@ -298,28 +313,13 @@
   </si>
   <si>
     <t>Z_GIVPR205</t>
-  </si>
-  <si>
-    <t>ETHIAS,PROVINCE LIEGE,AME-LIFE,NRB</t>
-  </si>
-  <si>
-    <t>ETHIAS,RESA,SIBELGA,PROVINCE LIEGE,AME-LIFE,NRB</t>
-  </si>
-  <si>
-    <t>ETHIAS,RESA,PROVINCE LIEGE,AME-LIFE,NRB</t>
-  </si>
-  <si>
-    <t>COMPANY_BREAKDOWN</t>
-  </si>
-  <si>
-    <t>RESA,IPEX,NRB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,11 +904,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1204,10 +1204,10 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -1228,7 +1228,7 @@
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1249,874 +1249,874 @@
         <v>4</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="H3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="O4" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="P4" t="s">
         <v>26</v>
       </c>
+      <c r="Q4" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="5" spans="1:17">
+      <c r="A5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
         <v>21</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>26</v>
+      <c r="O7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="8" spans="1:17">
+      <c r="A8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O14" t="s">
+        <v>25</v>
+      </c>
+      <c r="P14" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="C16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="G16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
         <v>22</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M16" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s">
+      <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O16" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>26</v>
+      <c r="P16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="17" spans="1:17">
+      <c r="A17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="G17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
         <v>21</v>
       </c>
-      <c r="M5" t="s">
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
         <v>22</v>
       </c>
-      <c r="N5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" t="s">
         <v>24</v>
       </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" t="s">
-        <v>93</v>
-      </c>
-      <c r="K7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="O17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17" t="s">
         <v>90</v>
       </c>
-      <c r="K10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" t="s">
-        <v>59</v>
-      </c>
-      <c r="O10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" t="s">
-        <v>64</v>
-      </c>
-      <c r="O11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" t="s">
-        <v>77</v>
-      </c>
-      <c r="O14" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O15" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" t="s">
-        <v>23</v>
-      </c>
-      <c r="O17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" t="s">
-        <v>85</v>
-      </c>
       <c r="Q17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2125,18 +2125,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2298,36 +2298,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B147D0-6BDF-40F0-BCE5-D9B832E09F65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D0389F-FE32-4930-9A10-415F18E77646}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D0389F-FE32-4930-9A10-415F18E77646}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B147D0-6BDF-40F0-BCE5-D9B832E09F65}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB7F80E-E117-40BE-90C7-323075F9B119}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="35a18e0c-895f-4e6d-96a9-0d0cdf6d7134"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB7F80E-E117-40BE-90C7-323075F9B119}"/>
 </file>
</xml_diff>